<commit_message>
Before changing test Cases
</commit_message>
<xml_diff>
--- a/Execute/Testing Execute Stage.xlsx
+++ b/Execute/Testing Execute Stage.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\CCE\Year 3 - Senior 1\Semester 2\Arch\Project\Repo\Architecture-Project\Execute\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24D7ED5B-0BC6-4B10-A1CE-07ED21B81121}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96AB6540-3A03-48B9-98CF-1D7C144B5B3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3F3EB091-F05C-4620-9C32-1374603C408F}"/>
   </bookViews>
@@ -262,9 +262,6 @@
     <t>"1_0_0_1_01_0110_00_0_0_0_0_0_0_0_0_0_0_0_0"</t>
   </si>
   <si>
-    <t>"1_0_0_0_01_0111_00_0_0_0_0_0_0_0_0_0_0_0_0"</t>
-  </si>
-  <si>
     <t>16#01214121</t>
   </si>
   <si>
@@ -317,6 +314,9 @@
   </si>
   <si>
     <t>16# F89ABCDE</t>
+  </si>
+  <si>
+    <t>"1_0_0_0_00_0111_00_0_0_0_0_0_0_0_0_0_0_0_0"</t>
   </si>
 </sst>
 </file>
@@ -799,8 +799,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E21ECAA5-5D80-48A2-BE22-2117CA212727}">
   <dimension ref="A1:AC19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W7" sqref="W7"/>
+    <sheetView tabSelected="1" topLeftCell="S3" workbookViewId="0">
+      <selection activeCell="Z3" sqref="Z3:Z34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1192,7 +1192,7 @@
         <v>0</v>
       </c>
       <c r="W5" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="X5" s="8" t="s">
         <v>55</v>
@@ -1278,7 +1278,7 @@
         <v>0</v>
       </c>
       <c r="W6" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="X6" s="8" t="s">
         <v>55</v>
@@ -1583,7 +1583,7 @@
         <v>51</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>75</v>
+        <v>93</v>
       </c>
       <c r="J10" s="8" t="s">
         <v>53</v>
@@ -1616,19 +1616,19 @@
         <v>68</v>
       </c>
       <c r="U10" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="V10" s="8">
+        <v>0</v>
+      </c>
+      <c r="W10" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="V10" s="8">
-        <v>0</v>
-      </c>
-      <c r="W10" s="8" t="s">
-        <v>76</v>
-      </c>
       <c r="X10" s="8" t="s">
         <v>55</v>
       </c>
       <c r="Y10" s="8" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="Z10" s="8">
         <v>0</v>
@@ -1657,7 +1657,7 @@
         <v>55</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F11" s="8" t="s">
         <v>49</v>
@@ -1669,7 +1669,7 @@
         <v>51</v>
       </c>
       <c r="I11" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J11" s="8" t="s">
         <v>53</v>
@@ -1699,16 +1699,16 @@
         <v>46</v>
       </c>
       <c r="T11" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="U11" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="V11" s="8">
         <v>0</v>
       </c>
       <c r="W11" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="X11" s="8" t="s">
         <v>55</v>
@@ -1743,7 +1743,7 @@
         <v>55</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F12" s="8" t="s">
         <v>49</v>
@@ -1755,7 +1755,7 @@
         <v>51</v>
       </c>
       <c r="I12" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J12" s="8" t="s">
         <v>53</v>
@@ -1785,10 +1785,10 @@
         <v>46</v>
       </c>
       <c r="T12" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="U12" s="8" t="s">
         <v>80</v>
-      </c>
-      <c r="U12" s="8" t="s">
-        <v>81</v>
       </c>
       <c r="V12" s="8">
         <v>0</v>
@@ -1823,7 +1823,7 @@
         <v>46</v>
       </c>
       <c r="T13" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="V13" s="8">
         <v>0</v>
@@ -1864,7 +1864,7 @@
         <v>55</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F14" s="8" t="s">
         <v>49</v>
@@ -1876,7 +1876,7 @@
         <v>51</v>
       </c>
       <c r="I14" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J14" s="8" t="s">
         <v>53</v>
@@ -1906,16 +1906,16 @@
         <v>46</v>
       </c>
       <c r="T14" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="U14" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="V14" s="8">
         <v>0</v>
       </c>
       <c r="W14" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="X14" s="8" t="s">
         <v>55</v>
@@ -1977,7 +1977,7 @@
         <v>0</v>
       </c>
       <c r="N15" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="O15" s="8" t="s">
         <v>48</v>
@@ -1992,7 +1992,7 @@
         <v>46</v>
       </c>
       <c r="T15" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="U15" s="8" t="s">
         <v>52</v>
@@ -2001,7 +2001,7 @@
         <v>0</v>
       </c>
       <c r="W15" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="X15" s="8" t="s">
         <v>55</v>
@@ -2048,7 +2048,7 @@
         <v>51</v>
       </c>
       <c r="I16" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J16" s="8" t="s">
         <v>49</v>
@@ -2063,31 +2063,31 @@
         <v>1</v>
       </c>
       <c r="N16" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="O16" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="P16" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q16" s="8">
+        <v>0</v>
+      </c>
+      <c r="S16" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="T16" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="U16" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="V16" s="8">
+        <v>0</v>
+      </c>
+      <c r="W16" s="8" t="s">
         <v>83</v>
-      </c>
-      <c r="O16" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="P16" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="Q16" s="8">
-        <v>0</v>
-      </c>
-      <c r="S16" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="T16" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="U16" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="V16" s="8">
-        <v>0</v>
-      </c>
-      <c r="W16" s="8" t="s">
-        <v>84</v>
       </c>
       <c r="X16" s="8" t="s">
         <v>55</v>
@@ -2149,10 +2149,10 @@
         <v>1</v>
       </c>
       <c r="N17" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="O17" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="P17" s="8" t="s">
         <v>48</v>
@@ -2164,7 +2164,7 @@
         <v>46</v>
       </c>
       <c r="T17" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="U17" s="8" t="s">
         <v>73</v>
@@ -2173,7 +2173,7 @@
         <v>0</v>
       </c>
       <c r="W17" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="X17" s="8" t="s">
         <v>55</v>
@@ -2220,7 +2220,7 @@
         <v>51</v>
       </c>
       <c r="I18" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J18" s="8" t="s">
         <v>49</v>
@@ -2235,46 +2235,46 @@
         <v>1</v>
       </c>
       <c r="N18" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="O18" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P18" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q18" s="8">
+        <v>0</v>
+      </c>
+      <c r="S18" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="T18" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="U18" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="V18" s="8">
+        <v>0</v>
+      </c>
+      <c r="W18" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="P18" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="Q18" s="8">
-        <v>0</v>
-      </c>
-      <c r="S18" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="T18" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="U18" s="8" t="s">
+      <c r="X18" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y18" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z18" s="8">
+        <v>0</v>
+      </c>
+      <c r="AA18" s="8">
+        <v>0</v>
+      </c>
+      <c r="AB18" s="8" t="s">
         <v>88</v>
-      </c>
-      <c r="V18" s="8">
-        <v>0</v>
-      </c>
-      <c r="W18" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="X18" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="Y18" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="Z18" s="8">
-        <v>0</v>
-      </c>
-      <c r="AA18" s="8">
-        <v>0</v>
-      </c>
-      <c r="AB18" s="8" t="s">
-        <v>89</v>
       </c>
       <c r="AC18" s="8" t="s">
         <v>53</v>
@@ -2306,7 +2306,7 @@
         <v>51</v>
       </c>
       <c r="I19" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J19" s="8" t="s">
         <v>49</v>
@@ -2321,49 +2321,49 @@
         <v>1</v>
       </c>
       <c r="N19" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="O19" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="P19" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="Q19" s="8">
         <v>1</v>
       </c>
       <c r="S19" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="T19" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="U19" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="V19" s="8">
+        <v>0</v>
+      </c>
+      <c r="W19" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="X19" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y19" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z19" s="8">
+        <v>0</v>
+      </c>
+      <c r="AA19" s="8">
+        <v>0</v>
+      </c>
+      <c r="AB19" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="V19" s="8">
-        <v>0</v>
-      </c>
-      <c r="W19" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="X19" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="Y19" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="Z19" s="8">
-        <v>0</v>
-      </c>
-      <c r="AA19" s="8">
-        <v>0</v>
-      </c>
-      <c r="AB19" s="8" t="s">
+      <c r="AC19" s="8" t="s">
         <v>89</v>
-      </c>
-      <c r="AC19" s="8" t="s">
-        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>